<commit_message>
WARNING - the commit for callback - Add code for LifeObjects
</commit_message>
<xml_diff>
--- a/Task4/Labyrinth/Roadmap.xlsx
+++ b/Task4/Labyrinth/Roadmap.xlsx
@@ -972,8 +972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>

</xml_diff>

<commit_message>
Add DeleteDeathObject() which delete actors with state isLive = false
</commit_message>
<xml_diff>
--- a/Task4/Labyrinth/Roadmap.xlsx
+++ b/Task4/Labyrinth/Roadmap.xlsx
@@ -69,9 +69,6 @@
     <t>Взаомодействие монстров и главного игрока</t>
   </si>
   <si>
-    <t>Ходит, стреляет</t>
-  </si>
-  <si>
     <t>Дойти до конца лабиринта</t>
   </si>
   <si>
@@ -135,13 +132,16 @@
     <t>В лабиринте будут расположены противники, игрок, стены, выход</t>
   </si>
   <si>
-    <t>Создание выходы из лабиринта</t>
-  </si>
-  <si>
     <t>Позиция противников задаётся в карте</t>
   </si>
   <si>
     <t>Позиция выхода и игрока задаётся в карте</t>
+  </si>
+  <si>
+    <t>Ходит, стреляет, пытается выйти из лабиринта</t>
+  </si>
+  <si>
+    <t>Создание выхода из лабиринта</t>
   </si>
 </sst>
 </file>
@@ -260,7 +260,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -303,6 +303,12 @@
         <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="22">
     <border>
@@ -590,7 +596,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -626,30 +632,18 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -688,6 +682,27 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -962,7 +977,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -972,8 +987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -989,25 +1004,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19.5" thickBot="1">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" s="25" t="s">
+      <c r="B1" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="G1" s="26"/>
+      <c r="G1" s="22"/>
     </row>
     <row r="2" spans="1:7" ht="20.25" thickTop="1" thickBot="1">
       <c r="A2" s="5" t="s">
@@ -1031,13 +1046,13 @@
         <v>3</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>4</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G3" s="10"/>
     </row>
@@ -1045,127 +1060,127 @@
       <c r="A4" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="14"/>
+    </row>
+    <row r="5" spans="1:7" ht="54">
+      <c r="A5" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C5" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" s="16"/>
+    </row>
+    <row r="6" spans="1:7" ht="36">
+      <c r="A6" s="24"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" s="16"/>
+    </row>
+    <row r="7" spans="1:7" ht="54">
+      <c r="A7" s="25"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="G4" s="15"/>
-    </row>
-    <row r="5" spans="1:7" ht="54">
-      <c r="A5" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="17" t="s">
+      <c r="D7" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="17" t="s">
+      <c r="E7" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="G5" s="18"/>
-    </row>
-    <row r="6" spans="1:7" ht="36">
-      <c r="A6" s="28"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="G6" s="18"/>
-    </row>
-    <row r="7" spans="1:7" ht="54">
-      <c r="A7" s="29"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="G7" s="22"/>
+      <c r="G7" s="18"/>
     </row>
     <row r="12" spans="1:7" ht="19.5" thickBot="1"/>
     <row r="13" spans="1:7" ht="19.5" thickBot="1">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="33" t="s">
+      <c r="B13" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="33"/>
+      <c r="C13" s="29"/>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="31"/>
+      <c r="B14" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="27"/>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="32"/>
+      <c r="C15" s="28"/>
     </row>
     <row r="17" spans="1:3" ht="19.5" thickBot="1"/>
     <row r="18" spans="1:3" ht="19.5" thickBot="1">
       <c r="A18" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="30" t="s">
+      <c r="B18" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="30"/>
+      <c r="C18" s="26"/>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="31"/>
+      <c r="C19" s="27"/>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="3"/>
-      <c r="B20" s="32"/>
-      <c r="C20" s="32"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
Add pause state. Update Roadmap.xlsx
</commit_message>
<xml_diff>
--- a/Task4/Labyrinth/Roadmap.xlsx
+++ b/Task4/Labyrinth/Roadmap.xlsx
@@ -662,6 +662,27 @@
     <xf numFmtId="0" fontId="14" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -682,27 +703,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -977,7 +977,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -987,8 +987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -1060,13 +1060,13 @@
       <c r="A4" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="24" t="s">
         <v>28</v>
       </c>
       <c r="E4" s="13" t="s">
@@ -1078,16 +1078,16 @@
       <c r="G4" s="14"/>
     </row>
     <row r="5" spans="1:7" ht="54">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="33" t="s">
+      <c r="D5" s="26" t="s">
         <v>29</v>
       </c>
       <c r="E5" s="15" t="s">
@@ -1099,13 +1099,13 @@
       <c r="G5" s="16"/>
     </row>
     <row r="6" spans="1:7" ht="36">
-      <c r="A6" s="24"/>
-      <c r="B6" s="32"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33" t="s">
+      <c r="A6" s="31"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="26" t="s">
         <v>32</v>
       </c>
       <c r="F6" s="15" t="s">
@@ -1114,12 +1114,12 @@
       <c r="G6" s="16"/>
     </row>
     <row r="7" spans="1:7" ht="54">
-      <c r="A7" s="25"/>
-      <c r="B7" s="34"/>
-      <c r="C7" s="35" t="s">
+      <c r="A7" s="32"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="36" t="s">
+      <c r="D7" s="29" t="s">
         <v>30</v>
       </c>
       <c r="E7" s="17" t="s">
@@ -1135,52 +1135,52 @@
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="29"/>
+      <c r="C13" s="36"/>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="27"/>
+      <c r="C14" s="34"/>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="28"/>
+      <c r="C15" s="35"/>
     </row>
     <row r="17" spans="1:3" ht="19.5" thickBot="1"/>
     <row r="18" spans="1:3" ht="19.5" thickBot="1">
       <c r="A18" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="26" t="s">
+      <c r="B18" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="26"/>
+      <c r="C18" s="33"/>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="27"/>
+      <c r="C19" s="34"/>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="3"/>
-      <c r="B20" s="28"/>
-      <c r="C20" s="28"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>